<commit_message>
fix(dificil ein): não é facil
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -29,13 +29,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Arial Black"/>
     </font>
     <font>
       <b/>
@@ -65,9 +68,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,16 +416,17 @@
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -432,7 +437,7 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>35</v>
       </c>
     </row>
@@ -443,7 +448,7 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>35</v>
       </c>
     </row>
@@ -454,7 +459,7 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>35</v>
       </c>
     </row>
@@ -465,7 +470,7 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>35</v>
       </c>
     </row>
@@ -476,7 +481,7 @@
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>35</v>
       </c>
     </row>
@@ -487,7 +492,7 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>35</v>
       </c>
     </row>
@@ -498,7 +503,7 @@
       <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>35</v>
       </c>
     </row>
@@ -509,7 +514,7 @@
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>35</v>
       </c>
     </row>

</xml_diff>